<commit_message>
feat(perf): show 10-frame avg IPC_Execute time in status bar
</commit_message>
<xml_diff>
--- a/doc/memo.xlsx
+++ b/doc/memo.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pekep\source\RawDxPlayerWpf\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468225C3-28A7-4329-A919-57F55612B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A4360-C130-45FD-9F3D-B5ACE44095F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3300" yWindow="3765" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
+    <workbookView xWindow="-20850" yWindow="3285" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
   </bookViews>
   <sheets>
     <sheet name="MainWindow" sheetId="1" r:id="rId1"/>
     <sheet name="RawFrameReader" sheetId="3" r:id="rId2"/>
     <sheet name="CudaInterop" sheetId="4" r:id="rId3"/>
-    <sheet name="DxRenderer" sheetId="2" r:id="rId4"/>
+    <sheet name="ImageProcCudaDLL" sheetId="5" r:id="rId4"/>
+    <sheet name="DxRenderer" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>MainWindow</t>
     <phoneticPr fontId="1"/>
@@ -316,6 +317,102 @@
   </si>
   <si>
     <t>CudaUnmapResources</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CudaProcessArrays_R16_To_BGRA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaCreateTextureObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaCreateSurfaceObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaDestroyTextureObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaGetLastError</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaDeviceSynchronize</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaDestroySurfaceObject</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sobel16Kernel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WLWWKernel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wlww_to_u8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>kernels</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaGraphicsUnmapResources(1, &amp;outRes, 0);</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ValidateParams</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CreateDeviceOnAdapterIndex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D3D11CreateDevice</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IPC_Init</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IPC_Shutdown</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OpenSharedResource</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CudaRegisterD3D11Texture(g_inputTex.Get(), &amp;g_cudaIn)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CudaRegisterD3D11Texture(g_outputTex.Get(), &amp;g_cudaOut)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IPC_SetParams</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IPC_Execute</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CudaUnregister(g_cudaOut)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CudaUnregister(g_cudaIn)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -367,7 +464,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1010,72 +1107,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4985467F-D7B1-4DDA-9E5E-1C75933DFC25}">
-  <dimension ref="Q6:R14"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="24.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="17" max="18" width="22.75" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="24.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="17:18" x14ac:dyDescent="0.4">
-      <c r="Q6" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="17:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="Q7" s="1" t="s">
+    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="17:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="Q8" s="1" t="s">
+    <row r="4" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="17:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="Q9" s="1" t="s">
+    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="17:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="R10" s="1" t="s">
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="17:18" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="R11" s="1" t="s">
+    <row r="7" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="17:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="R12" s="1" t="s">
+    <row r="8" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="17:18" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="R13" s="1" t="s">
+    <row r="9" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="17:18" x14ac:dyDescent="0.4">
-      <c r="Q14" s="1" t="s">
+    <row r="10" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B20" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1085,6 +1252,115 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D445E4E-BD7A-4F93-9635-C688573017FE}">
+  <dimension ref="E3:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="22" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="22" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="E4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="E6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="F7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="F8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="F9" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="F11" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="F12" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="E13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="E14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="F15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.4">
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="E17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="F18" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C7CE8C-B529-4BB5-9149-0E75F76583D9}">
   <dimension ref="B1:H17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix: adjust behavior based on old commit
</commit_message>
<xml_diff>
--- a/doc/memo.xlsx
+++ b/doc/memo.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pekep\source\RawDxPlayerWpf\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A4360-C130-45FD-9F3D-B5ACE44095F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0091305C-ADD0-4D99-AF29-4BBDE53D45C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20850" yWindow="3285" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
+    <workbookView xWindow="300" yWindow="2490" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
   </bookViews>
   <sheets>
     <sheet name="MainWindow" sheetId="1" r:id="rId1"/>
     <sheet name="RawFrameReader" sheetId="3" r:id="rId2"/>
     <sheet name="CudaInterop" sheetId="4" r:id="rId3"/>
     <sheet name="ImageProcCudaDLL" sheetId="5" r:id="rId4"/>
-    <sheet name="DxRenderer" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="DxRenderer" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="116">
   <si>
     <t>MainWindow</t>
     <phoneticPr fontId="1"/>
@@ -413,6 +414,93 @@
   </si>
   <si>
     <t>CudaUnregister(g_cudaIn)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_outputSharedHandle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IntPtr</t>
+  </si>
+  <si>
+    <t>IntPtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OutputSharedHandle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>public</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>private readonly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DxRenderer.cs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IImageProcessor.cs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>System.IntPtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>outputDxSharedHandle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NativeImageProcessor.cs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NativeImageProc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>outSharedHandle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>void*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g_outputTex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaGraphicsResource*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ComPtr&lt;ID3D11Texture2D&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>static</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g_cudaOut</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cudaGraphicsSubResourceGetMappedArray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>outArray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>void**</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1255,7 +1343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D445E4E-BD7A-4F93-9635-C688573017FE}">
   <dimension ref="E3:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1361,6 +1449,141 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727BFE05-5652-4318-BEC1-C3D671C00923}">
+  <dimension ref="A2:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.75" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="13.75" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C7CE8C-B529-4BB5-9149-0E75F76583D9}">
   <dimension ref="B1:H17"/>
   <sheetViews>

</xml_diff>

<commit_message>
- Removed DxRenderer and SharpDX dependency from WPF layer - Centralized D3D11 device and GPU resource management in native C++ code - Replaced shared texture based IO with D3D11 buffer based IO - Updated CUDA interop to use linear buffers instead of texture/array access - Added buffer-based upload, execute, and readback paths
</commit_message>
<xml_diff>
--- a/doc/memo.xlsx
+++ b/doc/memo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pekep\source\RawDxPlayerWpf\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0091305C-ADD0-4D99-AF29-4BBDE53D45C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F214F7FD-30CD-4073-88F4-702491FBFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2490" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
+    <workbookView xWindow="-25380" yWindow="0" windowWidth="21600" windowHeight="15585" activeTab="5" xr2:uid="{5B162454-BAF4-4998-8C24-16CB90E20D94}"/>
   </bookViews>
   <sheets>
     <sheet name="MainWindow" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="CudaInterop" sheetId="4" r:id="rId3"/>
     <sheet name="ImageProcCudaDLL" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
-    <sheet name="DxRenderer" sheetId="2" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
+    <sheet name="DxRenderer" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1452,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727BFE05-5652-4318-BEC1-C3D671C00923}">
   <dimension ref="A2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1584,6 +1585,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D3F51E-46A8-419D-B612-63D409B79AD9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B98" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="65.125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C7CE8C-B529-4BB5-9149-0E75F76583D9}">
   <dimension ref="B1:H17"/>
   <sheetViews>

</xml_diff>